<commit_message>
update optimization and using HiGHS solver
</commit_message>
<xml_diff>
--- a/output/summarise_per_nurse.xlsx
+++ b/output/summarise_per_nurse.xlsx
@@ -540,13 +540,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -554,22 +554,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -577,22 +577,22 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -600,22 +600,22 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -623,13 +623,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -638,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -646,13 +646,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -669,10 +669,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
         <v>7</v>
@@ -692,22 +692,22 @@
         <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
         <v>7</v>
       </c>
       <c r="D11" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -715,22 +715,22 @@
         <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
         <v>7</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -738,10 +738,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" t="n">
         <v>7</v>
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -761,19 +761,19 @@
         <v>10</v>
       </c>
       <c r="B14" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" t="n">
         <v>5</v>
       </c>
-      <c r="C14" t="n">
-        <v>6</v>
-      </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -784,13 +784,13 @@
         <v>11</v>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
         <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -830,10 +830,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
         <v>7</v>
@@ -842,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -853,19 +853,19 @@
         <v>14</v>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
         <v>6</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
         <v>1</v>
@@ -876,13 +876,13 @@
         <v>15</v>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -902,19 +902,19 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -922,22 +922,22 @@
         <v>17</v>
       </c>
       <c r="B21" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" t="n">
         <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -945,22 +945,22 @@
         <v>18</v>
       </c>
       <c r="B22" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -971,13 +971,13 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -991,22 +991,22 @@
         <v>20</v>
       </c>
       <c r="B24" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" t="n">
         <v>7</v>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1014,22 +1014,22 @@
         <v>21</v>
       </c>
       <c r="B25" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1040,19 +1040,19 @@
         <v>7</v>
       </c>
       <c r="C26" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1060,13 +1060,13 @@
         <v>23</v>
       </c>
       <c r="B27" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -1083,22 +1083,22 @@
         <v>24</v>
       </c>
       <c r="B28" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1106,22 +1106,22 @@
         <v>25</v>
       </c>
       <c r="B29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
         <v>7</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1138,10 +1138,10 @@
         <v>7</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1152,22 +1152,22 @@
         <v>27</v>
       </c>
       <c r="B31" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="n">
         <v>6</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1187,10 +1187,10 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1198,19 +1198,19 @@
         <v>29</v>
       </c>
       <c r="B33" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>

</xml_diff>